<commit_message>
Ajustes de nombres y términos
Cambio de títulos de recursos para evitar recursos diferentes con
nombres iguales, tanto en el Manuscrito como en el Esqueleto de guión.
Cambio del ítem “Imagen” por “Foto” en la hoja Cuaderno de estudios del
Esqueleto de guión.
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado04/guion01/EsqueletoGuion_MA_04_01_CO.xlsx
+++ b/fuentes/contenidos/grado04/guion01/EsqueletoGuion_MA_04_01_CO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johana Montejo Rozo\Dropbox\AULA PLANETA\Temas\Tema 1\Edición\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Documents\Aula Planeta Colombia\Repositorios\Matematicas\fuentes\contenidos\grado04\guion01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="729"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20492" windowHeight="7758" tabRatio="729"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="82">
   <si>
     <t>FICHA</t>
   </si>
@@ -171,9 +171,6 @@
     <t>Refuerza tu aprendizaje: Conjuntos</t>
   </si>
   <si>
-    <t>Colocar conjunto universal en la representación con Diagramas de Venn</t>
-  </si>
-  <si>
     <t>Mapa Conceptual</t>
   </si>
   <si>
@@ -186,9 +183,6 @@
     <t>Texto</t>
   </si>
   <si>
-    <t>Imagen</t>
-  </si>
-  <si>
     <t>Determinación de un conjunto por extensión</t>
   </si>
   <si>
@@ -276,7 +270,13 @@
     <t>Mapa conceptual</t>
   </si>
   <si>
-    <t>Webs de referencia</t>
+    <t>Foto</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: Analiza operaciones entre conjuntos</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: Identifica conjuntos</t>
   </si>
 </sst>
 </file>
@@ -343,7 +343,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -392,6 +392,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -833,7 +839,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -893,6 +899,7 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="401">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -1589,13 +1596,13 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="127.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.3984375" customWidth="1"/>
+    <col min="2" max="2" width="127.3984375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="13" t="s">
         <v>8</v>
       </c>
@@ -1603,7 +1610,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="13" t="s">
         <v>9</v>
       </c>
@@ -1611,7 +1618,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="13" t="s">
         <v>10</v>
       </c>
@@ -1619,7 +1626,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="13" t="s">
         <v>11</v>
       </c>
@@ -1627,7 +1634,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="13" t="s">
         <v>1</v>
       </c>
@@ -1635,7 +1642,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="13" t="s">
         <v>12</v>
       </c>
@@ -1662,19 +1669,19 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.7109375" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.73046875" customWidth="1"/>
+    <col min="5" max="5" width="20.3984375" customWidth="1"/>
+    <col min="7" max="7" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.73046875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
@@ -1694,7 +1701,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2"/>
@@ -1708,16 +1715,16 @@
       <c r="K2"/>
       <c r="L2"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="G12" s="8"/>
     </row>
   </sheetData>
@@ -1733,19 +1740,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:C22"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="66.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="66.1328125" customWidth="1"/>
+    <col min="2" max="2" width="14.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
@@ -1756,7 +1763,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1766,11 +1773,8 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1781,7 +1785,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -1792,7 +1796,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1803,7 +1807,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1814,7 +1818,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -1825,7 +1829,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
         <v>32</v>
       </c>
@@ -1836,7 +1840,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -1847,7 +1851,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
         <v>44</v>
       </c>
@@ -1858,7 +1862,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -1869,7 +1873,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -1880,7 +1884,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -1891,7 +1895,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -1902,7 +1906,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -1913,7 +1917,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
         <v>39</v>
       </c>
@@ -1924,7 +1928,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="4" t="s">
         <v>40</v>
       </c>
@@ -1935,7 +1939,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -1946,7 +1950,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -1957,9 +1961,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>43</v>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A20" s="31" t="s">
+        <v>80</v>
       </c>
       <c r="B20" t="s">
         <v>28</v>
@@ -1968,7 +1972,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -1979,7 +1983,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="4" t="s">
         <v>45</v>
       </c>
@@ -1990,9 +1994,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>45</v>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A23" s="31" t="s">
+        <v>81</v>
       </c>
       <c r="B23" t="s">
         <v>26</v>
@@ -2001,9 +2005,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B24" t="s">
         <v>26</v>
@@ -2012,9 +2016,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B25" t="s">
         <v>26</v>
@@ -2048,14 +2052,14 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="92.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.265625" customWidth="1"/>
+    <col min="3" max="3" width="19.265625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="23.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
@@ -2066,7 +2070,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2077,7 +2081,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2088,7 +2092,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2099,7 +2103,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2110,7 +2114,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2121,7 +2125,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2132,7 +2136,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2143,7 +2147,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2154,7 +2158,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2165,7 +2169,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2176,7 +2180,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2187,7 +2191,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2198,7 +2202,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2209,7 +2213,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2220,7 +2224,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2231,7 +2235,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2242,7 +2246,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2253,7 +2257,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2264,7 +2268,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2275,7 +2279,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2286,7 +2290,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2297,7 +2301,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2308,29 +2312,29 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C27" s="6"/>
     </row>
   </sheetData>
@@ -2350,24 +2354,24 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I61"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61:XFD61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="43.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="61.28515625" style="3" customWidth="1"/>
-    <col min="5" max="7" width="17.85546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="64.140625" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.1328125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="28.265625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="61.265625" style="3" customWidth="1"/>
+    <col min="5" max="7" width="17.86328125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="64.1328125" customWidth="1"/>
+    <col min="9" max="9" width="17.3984375" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="9" t="s">
         <v>6</v>
       </c>
@@ -2396,15 +2400,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>49</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>50</v>
       </c>
       <c r="D2" s="16"/>
       <c r="E2" s="16"/>
@@ -2413,15 +2417,15 @@
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="D3" s="16"/>
       <c r="E3" s="16"/>
@@ -2430,15 +2434,15 @@
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>49</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>50</v>
       </c>
       <c r="D4" s="16"/>
       <c r="E4" s="16"/>
@@ -2447,57 +2451,57 @@
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="16" t="s">
         <v>52</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>54</v>
       </c>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
@@ -2508,57 +2512,57 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
@@ -2569,57 +2573,57 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
@@ -2630,19 +2634,19 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
@@ -2653,15 +2657,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D15" s="19"/>
       <c r="E15" s="19"/>
@@ -2670,57 +2674,57 @@
       <c r="H15" s="17"/>
       <c r="I15" s="17"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C16" s="18"/>
       <c r="D16" s="19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F16" s="19"/>
       <c r="G16" s="19"/>
       <c r="H16" s="17"/>
       <c r="I16" s="17"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C17" s="18"/>
       <c r="D17" s="19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
       <c r="H17" s="17"/>
       <c r="I17" s="17"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C18" s="18"/>
       <c r="D18" s="19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F18" s="19"/>
       <c r="G18" s="19"/>
@@ -2731,19 +2735,19 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C19" s="18"/>
       <c r="D19" s="19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F19" s="19"/>
       <c r="G19" s="19"/>
@@ -2754,95 +2758,95 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C20" s="18"/>
       <c r="D20" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F20" s="19"/>
       <c r="G20" s="19"/>
       <c r="H20" s="17"/>
       <c r="I20" s="17"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C21" s="18"/>
       <c r="D21" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="F21" s="19"/>
       <c r="G21" s="19"/>
       <c r="H21" s="17"/>
       <c r="I21" s="17"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C22" s="18"/>
       <c r="D22" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F22" s="19"/>
       <c r="G22" s="19"/>
       <c r="H22" s="17"/>
       <c r="I22" s="17"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C23" s="18"/>
       <c r="D23" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F23" s="19"/>
       <c r="G23" s="19"/>
       <c r="H23" s="17"/>
       <c r="I23" s="17"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C24" s="18"/>
       <c r="D24" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F24" s="19"/>
       <c r="G24" s="19"/>
@@ -2853,61 +2857,61 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C25" s="18"/>
       <c r="D25" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F25" s="19"/>
       <c r="G25" s="19"/>
       <c r="H25" s="17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I25" s="17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C26" s="18"/>
       <c r="D26" s="19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F26" s="19"/>
       <c r="G26" s="19"/>
       <c r="H26" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="I26" s="17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A27" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="I26" s="17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" s="21" t="s">
-        <v>66</v>
-      </c>
       <c r="C27" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
@@ -2916,15 +2920,15 @@
       <c r="H27" s="20"/>
       <c r="I27" s="20"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
@@ -2937,57 +2941,57 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C29" s="21"/>
       <c r="D29" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
       <c r="H29" s="20"/>
       <c r="I29" s="20"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B30" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C30" s="21"/>
       <c r="D30" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F30" s="22"/>
       <c r="G30" s="22"/>
       <c r="H30" s="20"/>
       <c r="I30" s="20"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C31" s="21"/>
       <c r="D31" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F31" s="22"/>
       <c r="G31" s="22"/>
@@ -2998,57 +3002,57 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C32" s="21"/>
       <c r="D32" s="22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F32" s="22"/>
       <c r="G32" s="22"/>
       <c r="H32" s="20"/>
       <c r="I32" s="20"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C33" s="21"/>
       <c r="D33" s="22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F33" s="22"/>
       <c r="G33" s="22"/>
       <c r="H33" s="20"/>
       <c r="I33" s="20"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C34" s="21"/>
       <c r="D34" s="22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F34" s="22"/>
       <c r="G34" s="22"/>
@@ -3059,57 +3063,57 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C35" s="21"/>
       <c r="D35" s="22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F35" s="22"/>
       <c r="G35" s="22"/>
       <c r="H35" s="20"/>
       <c r="I35" s="20"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C36" s="21"/>
       <c r="D36" s="22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="F36" s="22"/>
       <c r="G36" s="22"/>
       <c r="H36" s="20"/>
       <c r="I36" s="20"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C37" s="21"/>
       <c r="D37" s="22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F37" s="22"/>
       <c r="G37" s="22"/>
@@ -3120,76 +3124,76 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C38" s="21"/>
       <c r="D38" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F38" s="22"/>
       <c r="G38" s="22"/>
       <c r="H38" s="20"/>
       <c r="I38" s="20"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C39" s="21"/>
       <c r="D39" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F39" s="22"/>
       <c r="G39" s="22"/>
       <c r="H39" s="20"/>
       <c r="I39" s="20"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A40" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C40" s="21"/>
       <c r="D40" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E40" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F40" s="22"/>
       <c r="G40" s="22"/>
       <c r="H40" s="20"/>
       <c r="I40" s="20"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C41" s="21"/>
       <c r="D41" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F41" s="22"/>
       <c r="G41" s="22"/>
@@ -3200,101 +3204,101 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C42" s="21"/>
       <c r="D42" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E42" s="22" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F42" s="22"/>
       <c r="G42" s="22"/>
       <c r="H42" s="20"/>
       <c r="I42" s="20"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C43" s="21"/>
       <c r="D43" s="22" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E43" s="22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F43" s="22"/>
       <c r="G43" s="22"/>
       <c r="H43" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="I43" s="20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A44" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B44" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C44" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D44" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="I43" s="20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="B44" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="C44" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="D44" s="25" t="s">
-        <v>73</v>
-      </c>
       <c r="E44" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F44" s="25"/>
       <c r="G44" s="25"/>
       <c r="H44" s="23"/>
       <c r="I44" s="23"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B45" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C45" s="24"/>
       <c r="D45" s="25" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E45" s="25" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="F45" s="25"/>
       <c r="G45" s="25"/>
       <c r="H45" s="23"/>
       <c r="I45" s="23"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A46" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B46" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C46" s="24"/>
       <c r="D46" s="25" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E46" s="25" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F46" s="25"/>
       <c r="G46" s="25"/>
@@ -3305,179 +3309,179 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B47" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C47" s="24"/>
       <c r="D47" s="25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E47" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F47" s="25"/>
       <c r="G47" s="25"/>
       <c r="H47" s="23"/>
       <c r="I47" s="23"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B48" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C48" s="24"/>
       <c r="D48" s="25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E48" s="25" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="F48" s="25"/>
       <c r="G48" s="25"/>
       <c r="H48" s="23"/>
       <c r="I48" s="23"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B49" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C49" s="24"/>
       <c r="D49" s="25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E49" s="25" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F49" s="25"/>
       <c r="G49" s="25"/>
       <c r="H49" s="23" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I49" s="23" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B50" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C50" s="24"/>
       <c r="D50" s="25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E50" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F50" s="25"/>
       <c r="G50" s="25"/>
       <c r="H50" s="23"/>
       <c r="I50" s="23"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B51" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C51" s="24"/>
       <c r="D51" s="25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E51" s="25" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="F51" s="25"/>
       <c r="G51" s="25"/>
       <c r="H51" s="23"/>
       <c r="I51" s="23"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B52" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C52" s="24"/>
       <c r="D52" s="25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E52" s="25" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="F52" s="25"/>
       <c r="G52" s="25"/>
       <c r="H52" s="23"/>
       <c r="I52" s="23"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A53" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B53" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C53" s="24"/>
       <c r="D53" s="25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E53" s="25" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F53" s="25"/>
       <c r="G53" s="25"/>
       <c r="H53" s="23"/>
       <c r="I53" s="23"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A54" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B54" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C54" s="24"/>
       <c r="D54" s="25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E54" s="25" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F54" s="25"/>
       <c r="G54" s="25"/>
       <c r="H54" s="23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I54" s="23" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A55" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B55" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C55" s="24"/>
       <c r="D55" s="25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E55" s="25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F55" s="25"/>
       <c r="G55" s="25"/>
@@ -3488,19 +3492,19 @@
         <v>26</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A56" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B56" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C56" s="24"/>
       <c r="D56" s="25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E56" s="25" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F56" s="25"/>
       <c r="G56" s="25"/>
@@ -3511,106 +3515,89 @@
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A57" s="26" t="s">
         <v>19</v>
       </c>
       <c r="B57" s="27" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C57" s="27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D57" s="28"/>
       <c r="E57" s="28"/>
       <c r="F57" s="28"/>
       <c r="G57" s="28"/>
       <c r="H57" s="26" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I57" s="26" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A58" s="26" t="s">
         <v>19</v>
       </c>
       <c r="B58" s="27" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C58" s="27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D58" s="28"/>
       <c r="E58" s="28"/>
       <c r="F58" s="28"/>
       <c r="G58" s="28"/>
       <c r="H58" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="I58" s="26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A59" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B59" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C59" s="29" t="s">
         <v>78</v>
-      </c>
-      <c r="I58" s="26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="B59" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="C59" s="29" t="s">
-        <v>80</v>
       </c>
       <c r="D59" s="30"/>
       <c r="E59" s="30"/>
       <c r="F59" s="30"/>
       <c r="G59" s="30"/>
       <c r="H59" s="29" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I59" s="29" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A60" s="29" t="s">
         <v>19</v>
       </c>
       <c r="B60" s="29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C60" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D60" s="30"/>
       <c r="E60" s="30"/>
       <c r="F60" s="30"/>
       <c r="G60" s="30"/>
       <c r="H60" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I60" s="29" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="B61" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="C61" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="D61" s="30"/>
-      <c r="E61" s="30"/>
-      <c r="F61" s="30"/>
-      <c r="G61" s="30"/>
-      <c r="H61" s="29"/>
-      <c r="I61" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ajuste de elementos según retroalimentación de GRECO
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado04/guion01/EsqueletoGuion_MA_04_01_CO.xlsx
+++ b/fuentes/contenidos/grado04/guion01/EsqueletoGuion_MA_04_01_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Documents\Aula Planeta Colombia\Repositorios\Matematicas\fuentes\contenidos\grado04\guion01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\Aula Planeta Colombia\Repositorios\Matematicas\fuentes\contenidos\grado04\guion01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="79">
   <si>
     <t>FICHA</t>
   </si>
@@ -159,9 +159,6 @@
     <t>Identifica los elementos de la intersección</t>
   </si>
   <si>
-    <t>Actividad para prcticar la diferencia entre conjuntos</t>
-  </si>
-  <si>
     <t>Refuerza tu aprendizaje: Operaciones entre conjuntos</t>
   </si>
   <si>
@@ -219,9 +216,6 @@
     <t>Recuerda</t>
   </si>
   <si>
-    <t xml:space="preserve">Refuerza tu aprendizaje: Relación de pertenencia y contenencia. </t>
-  </si>
-  <si>
     <t xml:space="preserve">¿Cuál conjunto está contenido? </t>
   </si>
   <si>
@@ -240,9 +234,6 @@
     <t>Conjunto vacío</t>
   </si>
   <si>
-    <t xml:space="preserve">Refuerza tu aprendizaje: Clasificación de conjuntos. </t>
-  </si>
-  <si>
     <t>Operaciones entre conjuntos</t>
   </si>
   <si>
@@ -252,18 +243,12 @@
     <t>Intersección entre conjuntos</t>
   </si>
   <si>
-    <t>Identifica los objetos de la intersección</t>
-  </si>
-  <si>
     <t>Diferencia entre conjuntos</t>
   </si>
   <si>
     <t>Ejercitación y competencias</t>
   </si>
   <si>
-    <t xml:space="preserve">Refuerza tu aprendizaje: Conjuntos. </t>
-  </si>
-  <si>
     <t>Fin de la unidad</t>
   </si>
   <si>
@@ -277,6 +262,12 @@
   </si>
   <si>
     <t>Refuerza tu aprendizaje: Identifica conjuntos</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: Clasificación de conjuntos</t>
+  </si>
+  <si>
+    <t>Actividad para practicar la diferencia entre conjuntos</t>
   </si>
 </sst>
 </file>
@@ -839,7 +830,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -900,6 +891,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="401">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -1743,7 +1735,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
@@ -1853,7 +1845,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>26</v>
@@ -1951,8 +1943,8 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>42</v>
+      <c r="A19" s="31" t="s">
+        <v>78</v>
       </c>
       <c r="B19" t="s">
         <v>26</v>
@@ -1963,7 +1955,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" s="31" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B20" t="s">
         <v>28</v>
@@ -1974,7 +1966,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B21" t="s">
         <v>26</v>
@@ -1985,7 +1977,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>26</v>
@@ -1996,7 +1988,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="31" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B23" t="s">
         <v>26</v>
@@ -2007,7 +1999,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B24" t="s">
         <v>26</v>
@@ -2018,7 +2010,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B25" t="s">
         <v>26</v>
@@ -2049,7 +2041,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
@@ -2163,7 +2155,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>26</v>
@@ -2261,8 +2253,8 @@
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>42</v>
+      <c r="B19" s="31" t="s">
+        <v>78</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>26</v>
@@ -2272,8 +2264,8 @@
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>43</v>
+      <c r="B20" s="31" t="s">
+        <v>75</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>26</v>
@@ -2284,7 +2276,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>26</v>
@@ -2295,7 +2287,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>26</v>
@@ -2305,8 +2297,8 @@
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>45</v>
+      <c r="B23" s="31" t="s">
+        <v>76</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>26</v>
@@ -2317,7 +2309,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>26</v>
@@ -2328,7 +2320,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>26</v>
@@ -2357,7 +2349,7 @@
   <dimension ref="A1:I60"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61:XFD61"/>
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
@@ -2405,10 +2397,10 @@
         <v>19</v>
       </c>
       <c r="B2" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>48</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>49</v>
       </c>
       <c r="D2" s="16"/>
       <c r="E2" s="16"/>
@@ -2422,10 +2414,10 @@
         <v>19</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D3" s="16"/>
       <c r="E3" s="16"/>
@@ -2439,10 +2431,10 @@
         <v>19</v>
       </c>
       <c r="B4" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>48</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>49</v>
       </c>
       <c r="D4" s="16"/>
       <c r="E4" s="16"/>
@@ -2456,14 +2448,14 @@
         <v>19</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
@@ -2475,14 +2467,14 @@
         <v>19</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="16" t="s">
         <v>50</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>51</v>
       </c>
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
@@ -2494,14 +2486,14 @@
         <v>19</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
@@ -2517,14 +2509,14 @@
         <v>19</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
@@ -2536,14 +2528,14 @@
         <v>19</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
@@ -2555,14 +2547,14 @@
         <v>19</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
@@ -2578,14 +2570,14 @@
         <v>19</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
@@ -2597,14 +2589,14 @@
         <v>19</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
@@ -2616,14 +2608,14 @@
         <v>19</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="16" t="s">
         <v>54</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>55</v>
       </c>
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
@@ -2639,14 +2631,14 @@
         <v>19</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
@@ -2662,10 +2654,10 @@
         <v>19</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D15" s="19"/>
       <c r="E15" s="19"/>
@@ -2679,14 +2671,14 @@
         <v>19</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C16" s="18"/>
       <c r="D16" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F16" s="19"/>
       <c r="G16" s="19"/>
@@ -2698,14 +2690,14 @@
         <v>19</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C17" s="18"/>
       <c r="D17" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
@@ -2717,14 +2709,14 @@
         <v>19</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C18" s="18"/>
       <c r="D18" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F18" s="19"/>
       <c r="G18" s="19"/>
@@ -2740,14 +2732,14 @@
         <v>19</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C19" s="18"/>
       <c r="D19" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F19" s="19"/>
       <c r="G19" s="19"/>
@@ -2763,14 +2755,14 @@
         <v>19</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C20" s="18"/>
       <c r="D20" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F20" s="19"/>
       <c r="G20" s="19"/>
@@ -2782,14 +2774,14 @@
         <v>19</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C21" s="18"/>
       <c r="D21" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F21" s="19"/>
       <c r="G21" s="19"/>
@@ -2801,14 +2793,14 @@
         <v>19</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C22" s="18"/>
       <c r="D22" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="19" t="s">
         <v>59</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>60</v>
       </c>
       <c r="F22" s="19"/>
       <c r="G22" s="19"/>
@@ -2820,14 +2812,14 @@
         <v>19</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C23" s="18"/>
       <c r="D23" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F23" s="19"/>
       <c r="G23" s="19"/>
@@ -2839,14 +2831,14 @@
         <v>19</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C24" s="18"/>
       <c r="D24" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F24" s="19"/>
       <c r="G24" s="19"/>
@@ -2862,19 +2854,19 @@
         <v>19</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C25" s="18"/>
       <c r="D25" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F25" s="19"/>
       <c r="G25" s="19"/>
       <c r="H25" s="17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I25" s="17" t="s">
         <v>26</v>
@@ -2885,19 +2877,19 @@
         <v>19</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C26" s="18"/>
       <c r="D26" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F26" s="19"/>
       <c r="G26" s="19"/>
-      <c r="H26" s="17" t="s">
-        <v>62</v>
+      <c r="H26" s="32" t="s">
+        <v>43</v>
       </c>
       <c r="I26" s="17" t="s">
         <v>26</v>
@@ -2908,10 +2900,10 @@
         <v>19</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
@@ -2925,10 +2917,10 @@
         <v>19</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
@@ -2946,14 +2938,14 @@
         <v>19</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C29" s="21"/>
       <c r="D29" s="22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
@@ -2965,14 +2957,14 @@
         <v>19</v>
       </c>
       <c r="B30" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C30" s="21"/>
       <c r="D30" s="22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F30" s="22"/>
       <c r="G30" s="22"/>
@@ -2984,14 +2976,14 @@
         <v>19</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C31" s="21"/>
       <c r="D31" s="22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F31" s="22"/>
       <c r="G31" s="22"/>
@@ -3007,14 +2999,14 @@
         <v>19</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C32" s="21"/>
       <c r="D32" s="22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F32" s="22"/>
       <c r="G32" s="22"/>
@@ -3026,14 +3018,14 @@
         <v>19</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C33" s="21"/>
       <c r="D33" s="22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F33" s="22"/>
       <c r="G33" s="22"/>
@@ -3045,14 +3037,14 @@
         <v>19</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C34" s="21"/>
       <c r="D34" s="22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F34" s="22"/>
       <c r="G34" s="22"/>
@@ -3068,14 +3060,14 @@
         <v>19</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C35" s="21"/>
       <c r="D35" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F35" s="22"/>
       <c r="G35" s="22"/>
@@ -3087,14 +3079,14 @@
         <v>19</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C36" s="21"/>
       <c r="D36" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F36" s="22"/>
       <c r="G36" s="22"/>
@@ -3106,14 +3098,14 @@
         <v>19</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C37" s="21"/>
       <c r="D37" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F37" s="22"/>
       <c r="G37" s="22"/>
@@ -3129,14 +3121,14 @@
         <v>19</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C38" s="21"/>
       <c r="D38" s="22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F38" s="22"/>
       <c r="G38" s="22"/>
@@ -3148,14 +3140,14 @@
         <v>19</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C39" s="21"/>
       <c r="D39" s="22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F39" s="22"/>
       <c r="G39" s="22"/>
@@ -3167,14 +3159,14 @@
         <v>19</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C40" s="21"/>
       <c r="D40" s="22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E40" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F40" s="22"/>
       <c r="G40" s="22"/>
@@ -3186,14 +3178,14 @@
         <v>19</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C41" s="21"/>
       <c r="D41" s="22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F41" s="22"/>
       <c r="G41" s="22"/>
@@ -3209,14 +3201,14 @@
         <v>19</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C42" s="21"/>
       <c r="D42" s="22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E42" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F42" s="22"/>
       <c r="G42" s="22"/>
@@ -3228,19 +3220,19 @@
         <v>19</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C43" s="21"/>
       <c r="D43" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E43" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F43" s="22"/>
       <c r="G43" s="22"/>
-      <c r="H43" s="20" t="s">
-        <v>69</v>
+      <c r="H43" s="32" t="s">
+        <v>77</v>
       </c>
       <c r="I43" s="20" t="s">
         <v>26</v>
@@ -3251,16 +3243,16 @@
         <v>19</v>
       </c>
       <c r="B44" s="24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C44" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D44" s="25" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E44" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F44" s="25"/>
       <c r="G44" s="25"/>
@@ -3272,14 +3264,14 @@
         <v>19</v>
       </c>
       <c r="B45" s="24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C45" s="24"/>
       <c r="D45" s="25" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E45" s="25" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F45" s="25"/>
       <c r="G45" s="25"/>
@@ -3291,14 +3283,14 @@
         <v>19</v>
       </c>
       <c r="B46" s="24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C46" s="24"/>
       <c r="D46" s="25" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E46" s="25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F46" s="25"/>
       <c r="G46" s="25"/>
@@ -3314,14 +3306,14 @@
         <v>19</v>
       </c>
       <c r="B47" s="24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C47" s="24"/>
       <c r="D47" s="25" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E47" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F47" s="25"/>
       <c r="G47" s="25"/>
@@ -3333,14 +3325,14 @@
         <v>19</v>
       </c>
       <c r="B48" s="24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C48" s="24"/>
       <c r="D48" s="25" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E48" s="25" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F48" s="25"/>
       <c r="G48" s="25"/>
@@ -3352,19 +3344,19 @@
         <v>19</v>
       </c>
       <c r="B49" s="24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C49" s="24"/>
       <c r="D49" s="25" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E49" s="25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F49" s="25"/>
       <c r="G49" s="25"/>
-      <c r="H49" s="23" t="s">
-        <v>73</v>
+      <c r="H49" s="32" t="s">
+        <v>41</v>
       </c>
       <c r="I49" s="23" t="s">
         <v>26</v>
@@ -3375,14 +3367,14 @@
         <v>19</v>
       </c>
       <c r="B50" s="24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C50" s="24"/>
       <c r="D50" s="25" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E50" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F50" s="25"/>
       <c r="G50" s="25"/>
@@ -3394,14 +3386,14 @@
         <v>19</v>
       </c>
       <c r="B51" s="24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C51" s="24"/>
       <c r="D51" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="E51" s="25" t="s">
         <v>74</v>
-      </c>
-      <c r="E51" s="25" t="s">
-        <v>79</v>
       </c>
       <c r="F51" s="25"/>
       <c r="G51" s="25"/>
@@ -3413,14 +3405,14 @@
         <v>19</v>
       </c>
       <c r="B52" s="24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C52" s="24"/>
       <c r="D52" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="E52" s="25" t="s">
         <v>74</v>
-      </c>
-      <c r="E52" s="25" t="s">
-        <v>79</v>
       </c>
       <c r="F52" s="25"/>
       <c r="G52" s="25"/>
@@ -3432,14 +3424,14 @@
         <v>19</v>
       </c>
       <c r="B53" s="24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C53" s="24"/>
       <c r="D53" s="25" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E53" s="25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F53" s="25"/>
       <c r="G53" s="25"/>
@@ -3451,19 +3443,19 @@
         <v>19</v>
       </c>
       <c r="B54" s="24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C54" s="24"/>
       <c r="D54" s="25" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E54" s="25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F54" s="25"/>
       <c r="G54" s="25"/>
-      <c r="H54" s="23" t="s">
-        <v>74</v>
+      <c r="H54" s="32" t="s">
+        <v>78</v>
       </c>
       <c r="I54" s="23" t="s">
         <v>26</v>
@@ -3474,19 +3466,19 @@
         <v>19</v>
       </c>
       <c r="B55" s="24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C55" s="24"/>
       <c r="D55" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E55" s="25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F55" s="25"/>
       <c r="G55" s="25"/>
-      <c r="H55" s="23" t="s">
-        <v>43</v>
+      <c r="H55" s="32" t="s">
+        <v>75</v>
       </c>
       <c r="I55" s="25" t="s">
         <v>26</v>
@@ -3497,19 +3489,19 @@
         <v>19</v>
       </c>
       <c r="B56" s="24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C56" s="24"/>
       <c r="D56" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E56" s="25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F56" s="25"/>
       <c r="G56" s="25"/>
       <c r="H56" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I56" s="25" t="s">
         <v>26</v>
@@ -3520,17 +3512,17 @@
         <v>19</v>
       </c>
       <c r="B57" s="27" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C57" s="27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D57" s="28"/>
       <c r="E57" s="28"/>
       <c r="F57" s="28"/>
       <c r="G57" s="28"/>
       <c r="H57" s="26" t="s">
-        <v>76</v>
+        <v>44</v>
       </c>
       <c r="I57" s="26" t="s">
         <v>26</v>
@@ -3541,16 +3533,16 @@
         <v>19</v>
       </c>
       <c r="B58" s="27" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C58" s="27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D58" s="28"/>
       <c r="E58" s="28"/>
       <c r="F58" s="28"/>
       <c r="G58" s="28"/>
-      <c r="H58" s="26" t="s">
+      <c r="H58" s="32" t="s">
         <v>76</v>
       </c>
       <c r="I58" s="26" t="s">
@@ -3562,17 +3554,17 @@
         <v>19</v>
       </c>
       <c r="B59" s="29" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C59" s="29" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D59" s="30"/>
       <c r="E59" s="30"/>
       <c r="F59" s="30"/>
       <c r="G59" s="30"/>
       <c r="H59" s="29" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="I59" s="29" t="s">
         <v>26</v>
@@ -3583,17 +3575,17 @@
         <v>19</v>
       </c>
       <c r="B60" s="29" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C60" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D60" s="30"/>
       <c r="E60" s="30"/>
       <c r="F60" s="30"/>
       <c r="G60" s="30"/>
       <c r="H60" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I60" s="29" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
MA0401: Actualización de archivos
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado04/guion01/EsqueletoGuion_MA_04_01_CO.xlsx
+++ b/fuentes/contenidos/grado04/guion01/EsqueletoGuion_MA_04_01_CO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\Aula Planeta Colombia\Repositorios\Matematicas\fuentes\contenidos\grado04\guion01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Copia\JOHANNA\Documents\Documents\Matematicas\fuentes\contenidos\grado04\guion01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20492" windowHeight="7758" tabRatio="729"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="729" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="CUADERNO DEL PROFESOR" sheetId="15" r:id="rId4"/>
     <sheet name="CUADERNO DE ESTUDIO" sheetId="16" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="84">
   <si>
     <t>FICHA</t>
   </si>
@@ -159,6 +159,9 @@
     <t>Identifica los elementos de la intersección</t>
   </si>
   <si>
+    <t>Actividad para prcticar la diferencia entre conjuntos</t>
+  </si>
+  <si>
     <t>Refuerza tu aprendizaje: Operaciones entre conjuntos</t>
   </si>
   <si>
@@ -216,6 +219,9 @@
     <t>Recuerda</t>
   </si>
   <si>
+    <t xml:space="preserve">Refuerza tu aprendizaje: Relación de pertenencia y contenencia. </t>
+  </si>
+  <si>
     <t xml:space="preserve">¿Cuál conjunto está contenido? </t>
   </si>
   <si>
@@ -234,6 +240,9 @@
     <t>Conjunto vacío</t>
   </si>
   <si>
+    <t xml:space="preserve">Refuerza tu aprendizaje: Clasificación de conjuntos. </t>
+  </si>
+  <si>
     <t>Operaciones entre conjuntos</t>
   </si>
   <si>
@@ -243,12 +252,18 @@
     <t>Intersección entre conjuntos</t>
   </si>
   <si>
+    <t>Identifica los objetos de la intersección</t>
+  </si>
+  <si>
     <t>Diferencia entre conjuntos</t>
   </si>
   <si>
     <t>Ejercitación y competencias</t>
   </si>
   <si>
+    <t xml:space="preserve">Refuerza tu aprendizaje: Conjuntos. </t>
+  </si>
+  <si>
     <t>Fin de la unidad</t>
   </si>
   <si>
@@ -264,10 +279,10 @@
     <t>Refuerza tu aprendizaje: Identifica conjuntos</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: Clasificación de conjuntos</t>
-  </si>
-  <si>
-    <t>Actividad para practicar la diferencia entre conjuntos</t>
+    <t>Resuelve problemas aplicando operaciones entre conjuntos.</t>
+  </si>
+  <si>
+    <t>Refiuerza tu aprendizaje: Resuelve problemas aplicando operaciones entre conjuntos.</t>
   </si>
 </sst>
 </file>
@@ -830,7 +845,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -891,7 +906,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="401">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -1584,17 +1598,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.3984375" customWidth="1"/>
-    <col min="2" max="2" width="127.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="127.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>8</v>
       </c>
@@ -1602,7 +1616,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>9</v>
       </c>
@@ -1610,7 +1624,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>10</v>
       </c>
@@ -1618,7 +1632,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>11</v>
       </c>
@@ -1626,7 +1640,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>1</v>
       </c>
@@ -1634,7 +1648,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>12</v>
       </c>
@@ -1661,19 +1675,19 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.73046875" customWidth="1"/>
-    <col min="5" max="5" width="20.3984375" customWidth="1"/>
-    <col min="7" max="7" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.1328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.73046875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
@@ -1693,7 +1707,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2"/>
@@ -1707,16 +1721,16 @@
       <c r="K2"/>
       <c r="L2"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G12" s="8"/>
     </row>
   </sheetData>
@@ -1732,19 +1746,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="66.1328125" customWidth="1"/>
-    <col min="2" max="2" width="14.73046875" customWidth="1"/>
+    <col min="1" max="1" width="78.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
@@ -1755,7 +1769,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1766,7 +1780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1777,7 +1791,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -1788,7 +1802,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1799,7 +1813,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1810,7 +1824,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -1821,7 +1835,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>32</v>
       </c>
@@ -1832,7 +1846,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -1843,9 +1857,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>26</v>
@@ -1854,7 +1868,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -1865,7 +1879,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -1876,7 +1890,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -1887,7 +1901,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -1898,7 +1912,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -1909,7 +1923,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>39</v>
       </c>
@@ -1920,7 +1934,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>40</v>
       </c>
@@ -1931,7 +1945,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -1942,9 +1956,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A19" s="31" t="s">
-        <v>78</v>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>42</v>
       </c>
       <c r="B19" t="s">
         <v>26</v>
@@ -1953,9 +1967,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B20" t="s">
         <v>28</v>
@@ -1964,9 +1978,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B21" t="s">
         <v>26</v>
@@ -1975,31 +1989,31 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A22" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="4">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A23" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="B23" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="4">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
-        <v>45</v>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="31" t="s">
+        <v>81</v>
       </c>
       <c r="B24" t="s">
         <v>26</v>
@@ -2008,7 +2022,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -2017,6 +2031,17 @@
       </c>
       <c r="C25">
         <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -2024,7 +2049,7 @@
     <sortCondition ref="C2:C65"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2041,17 +2066,17 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="92.265625" customWidth="1"/>
-    <col min="3" max="3" width="19.265625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
@@ -2062,7 +2087,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2073,7 +2098,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2084,7 +2109,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2095,7 +2120,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2106,7 +2131,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2117,7 +2142,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2128,7 +2153,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2139,7 +2164,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2150,18 +2175,18 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2172,7 +2197,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2183,7 +2208,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2194,7 +2219,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2205,7 +2230,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2216,7 +2241,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2227,7 +2252,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2238,7 +2263,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2249,84 +2274,84 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="31" t="s">
-        <v>78</v>
+      <c r="B19" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="31" t="s">
-        <v>75</v>
+      <c r="B20" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="31" t="s">
-        <v>76</v>
+      <c r="B23" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C27" s="6"/>
     </row>
   </sheetData>
@@ -2346,24 +2371,24 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.73046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.1328125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="28.265625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="61.265625" style="3" customWidth="1"/>
-    <col min="5" max="7" width="17.86328125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="64.1328125" customWidth="1"/>
-    <col min="9" max="9" width="17.3984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="61.28515625" style="3" customWidth="1"/>
+    <col min="5" max="7" width="17.85546875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="64.140625" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>6</v>
       </c>
@@ -2392,15 +2417,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D2" s="16"/>
       <c r="E2" s="16"/>
@@ -2409,15 +2434,15 @@
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D3" s="16"/>
       <c r="E3" s="16"/>
@@ -2426,15 +2451,15 @@
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D4" s="16"/>
       <c r="E4" s="16"/>
@@ -2443,57 +2468,57 @@
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="16" t="s">
         <v>49</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>48</v>
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="16" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="16" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
@@ -2504,57 +2529,57 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="16" t="s">
         <v>52</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>51</v>
       </c>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
@@ -2565,57 +2590,57 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
@@ -2626,19 +2651,19 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="16" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
@@ -2649,15 +2674,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D15" s="19"/>
       <c r="E15" s="19"/>
@@ -2666,57 +2691,57 @@
       <c r="H15" s="17"/>
       <c r="I15" s="17"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C16" s="18"/>
       <c r="D16" s="19" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F16" s="19"/>
       <c r="G16" s="19"/>
       <c r="H16" s="17"/>
       <c r="I16" s="17"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C17" s="18"/>
       <c r="D17" s="19" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
       <c r="H17" s="17"/>
       <c r="I17" s="17"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C18" s="18"/>
       <c r="D18" s="19" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F18" s="19"/>
       <c r="G18" s="19"/>
@@ -2727,19 +2752,19 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C19" s="18"/>
       <c r="D19" s="19" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F19" s="19"/>
       <c r="G19" s="19"/>
@@ -2750,95 +2775,95 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C20" s="18"/>
       <c r="D20" s="19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F20" s="19"/>
       <c r="G20" s="19"/>
       <c r="H20" s="17"/>
       <c r="I20" s="17"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C21" s="18"/>
       <c r="D21" s="19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="F21" s="19"/>
       <c r="G21" s="19"/>
       <c r="H21" s="17"/>
       <c r="I21" s="17"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C22" s="18"/>
       <c r="D22" s="19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F22" s="19"/>
       <c r="G22" s="19"/>
       <c r="H22" s="17"/>
       <c r="I22" s="17"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C23" s="18"/>
       <c r="D23" s="19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F23" s="19"/>
       <c r="G23" s="19"/>
       <c r="H23" s="17"/>
       <c r="I23" s="17"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C24" s="18"/>
       <c r="D24" s="19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F24" s="19"/>
       <c r="G24" s="19"/>
@@ -2849,61 +2874,61 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C25" s="18"/>
       <c r="D25" s="19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F25" s="19"/>
       <c r="G25" s="19"/>
       <c r="H25" s="17" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I25" s="17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C26" s="18"/>
       <c r="D26" s="19" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F26" s="19"/>
       <c r="G26" s="19"/>
-      <c r="H26" s="32" t="s">
-        <v>43</v>
+      <c r="H26" s="17" t="s">
+        <v>62</v>
       </c>
       <c r="I26" s="17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
@@ -2912,15 +2937,15 @@
       <c r="H27" s="20"/>
       <c r="I27" s="20"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
@@ -2933,57 +2958,57 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C29" s="21"/>
       <c r="D29" s="22" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
       <c r="H29" s="20"/>
       <c r="I29" s="20"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B30" s="21" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C30" s="21"/>
       <c r="D30" s="22" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F30" s="22"/>
       <c r="G30" s="22"/>
       <c r="H30" s="20"/>
       <c r="I30" s="20"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C31" s="21"/>
       <c r="D31" s="22" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F31" s="22"/>
       <c r="G31" s="22"/>
@@ -2994,57 +3019,57 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C32" s="21"/>
       <c r="D32" s="22" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F32" s="22"/>
       <c r="G32" s="22"/>
       <c r="H32" s="20"/>
       <c r="I32" s="20"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C33" s="21"/>
       <c r="D33" s="22" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F33" s="22"/>
       <c r="G33" s="22"/>
       <c r="H33" s="20"/>
       <c r="I33" s="20"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C34" s="21"/>
       <c r="D34" s="22" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F34" s="22"/>
       <c r="G34" s="22"/>
@@ -3055,57 +3080,57 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C35" s="21"/>
       <c r="D35" s="22" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F35" s="22"/>
       <c r="G35" s="22"/>
       <c r="H35" s="20"/>
       <c r="I35" s="20"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C36" s="21"/>
       <c r="D36" s="22" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="F36" s="22"/>
       <c r="G36" s="22"/>
       <c r="H36" s="20"/>
       <c r="I36" s="20"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C37" s="21"/>
       <c r="D37" s="22" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F37" s="22"/>
       <c r="G37" s="22"/>
@@ -3116,76 +3141,76 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C38" s="21"/>
       <c r="D38" s="22" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F38" s="22"/>
       <c r="G38" s="22"/>
       <c r="H38" s="20"/>
       <c r="I38" s="20"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C39" s="21"/>
       <c r="D39" s="22" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F39" s="22"/>
       <c r="G39" s="22"/>
       <c r="H39" s="20"/>
       <c r="I39" s="20"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C40" s="21"/>
       <c r="D40" s="22" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E40" s="22" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F40" s="22"/>
       <c r="G40" s="22"/>
       <c r="H40" s="20"/>
       <c r="I40" s="20"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C41" s="21"/>
       <c r="D41" s="22" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F41" s="22"/>
       <c r="G41" s="22"/>
@@ -3196,101 +3221,101 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C42" s="21"/>
       <c r="D42" s="22" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E42" s="22" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F42" s="22"/>
       <c r="G42" s="22"/>
       <c r="H42" s="20"/>
       <c r="I42" s="20"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C43" s="21"/>
       <c r="D43" s="22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E43" s="22" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F43" s="22"/>
       <c r="G43" s="22"/>
-      <c r="H43" s="32" t="s">
-        <v>77</v>
+      <c r="H43" s="20" t="s">
+        <v>69</v>
       </c>
       <c r="I43" s="20" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B44" s="24" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C44" s="24" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D44" s="25" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E44" s="25" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F44" s="25"/>
       <c r="G44" s="25"/>
       <c r="H44" s="23"/>
       <c r="I44" s="23"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B45" s="24" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C45" s="24"/>
       <c r="D45" s="25" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E45" s="25" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="F45" s="25"/>
       <c r="G45" s="25"/>
       <c r="H45" s="23"/>
       <c r="I45" s="23"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B46" s="24" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C46" s="24"/>
       <c r="D46" s="25" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E46" s="25" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F46" s="25"/>
       <c r="G46" s="25"/>
@@ -3301,293 +3326,333 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B47" s="24" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C47" s="24"/>
       <c r="D47" s="25" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E47" s="25" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F47" s="25"/>
       <c r="G47" s="25"/>
       <c r="H47" s="23"/>
       <c r="I47" s="23"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B48" s="24" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C48" s="24"/>
       <c r="D48" s="25" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E48" s="25" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="F48" s="25"/>
       <c r="G48" s="25"/>
       <c r="H48" s="23"/>
       <c r="I48" s="23"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B49" s="24" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C49" s="24"/>
       <c r="D49" s="25" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E49" s="25" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F49" s="25"/>
       <c r="G49" s="25"/>
-      <c r="H49" s="32" t="s">
-        <v>41</v>
+      <c r="H49" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="I49" s="23" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B50" s="24" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C50" s="24"/>
       <c r="D50" s="25" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E50" s="25" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F50" s="25"/>
       <c r="G50" s="25"/>
       <c r="H50" s="23"/>
       <c r="I50" s="23"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B51" s="24" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C51" s="24"/>
       <c r="D51" s="25" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E51" s="25" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="F51" s="25"/>
       <c r="G51" s="25"/>
       <c r="H51" s="23"/>
       <c r="I51" s="23"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B52" s="24" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C52" s="24"/>
       <c r="D52" s="25" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E52" s="25" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="F52" s="25"/>
       <c r="G52" s="25"/>
       <c r="H52" s="23"/>
       <c r="I52" s="23"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B53" s="24" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C53" s="24"/>
       <c r="D53" s="25" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E53" s="25" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F53" s="25"/>
       <c r="G53" s="25"/>
       <c r="H53" s="23"/>
       <c r="I53" s="23"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B54" s="24" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C54" s="24"/>
       <c r="D54" s="25" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E54" s="25" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="F54" s="25"/>
       <c r="G54" s="25"/>
-      <c r="H54" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="I54" s="23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H54" s="23"/>
+      <c r="I54" s="23"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B55" s="24" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C55" s="24"/>
       <c r="D55" s="25" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="E55" s="25" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F55" s="25"/>
       <c r="G55" s="25"/>
-      <c r="H55" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="I55" s="25" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H55" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="I55" s="23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B56" s="24" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C56" s="24"/>
       <c r="D56" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="E56" s="25" t="s">
         <v>55</v>
-      </c>
-      <c r="E56" s="25" t="s">
-        <v>51</v>
       </c>
       <c r="F56" s="25"/>
       <c r="G56" s="25"/>
       <c r="H56" s="23" t="s">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="I56" s="25" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A57" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="B57" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="C57" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="D57" s="28"/>
-      <c r="E57" s="28"/>
-      <c r="F57" s="28"/>
-      <c r="G57" s="28"/>
-      <c r="H57" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="I57" s="26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A58" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="B58" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="C58" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="D58" s="28"/>
-      <c r="E58" s="28"/>
-      <c r="F58" s="28"/>
-      <c r="G58" s="28"/>
-      <c r="H58" s="32" t="s">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B57" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C57" s="24"/>
+      <c r="D57" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="E57" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="F57" s="25"/>
+      <c r="G57" s="25"/>
+      <c r="H57" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="I57" s="25"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B58" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C58" s="24"/>
+      <c r="D58" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="E58" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="F58" s="25"/>
+      <c r="G58" s="25"/>
+      <c r="H58" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="I58" s="25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B59" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="C59" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="D59" s="28"/>
+      <c r="E59" s="28"/>
+      <c r="F59" s="28"/>
+      <c r="G59" s="28"/>
+      <c r="H59" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="I58" s="26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A59" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="B59" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="C59" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="D59" s="30"/>
-      <c r="E59" s="30"/>
-      <c r="F59" s="30"/>
-      <c r="G59" s="30"/>
-      <c r="H59" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="I59" s="29" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A60" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="B60" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="C60" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="D60" s="30"/>
-      <c r="E60" s="30"/>
-      <c r="F60" s="30"/>
-      <c r="G60" s="30"/>
-      <c r="H60" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="I60" s="29" t="s">
+      <c r="I59" s="26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B60" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="C60" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="D60" s="28"/>
+      <c r="E60" s="28"/>
+      <c r="F60" s="28"/>
+      <c r="G60" s="28"/>
+      <c r="H60" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="I60" s="26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B61" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C61" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="D61" s="30"/>
+      <c r="E61" s="30"/>
+      <c r="F61" s="30"/>
+      <c r="G61" s="30"/>
+      <c r="H61" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="I61" s="29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B62" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C62" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="D62" s="30"/>
+      <c r="E62" s="30"/>
+      <c r="F62" s="30"/>
+      <c r="G62" s="30"/>
+      <c r="H62" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="I62" s="29" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
MA0401: Esqueleto aprobado por España
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado04/guion01/EsqueletoGuion_MA_04_01_CO.xlsx
+++ b/fuentes/contenidos/grado04/guion01/EsqueletoGuion_MA_04_01_CO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Copia\JOHANNA\Documents\Documents\Matematicas\fuentes\contenidos\grado04\guion01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\Aula Planeta Colombia\Repositorios\Matematicas\fuentes\contenidos\grado04\guion01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="729" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20492" windowHeight="7758" tabRatio="729"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="CUADERNO DEL PROFESOR" sheetId="15" r:id="rId4"/>
     <sheet name="CUADERNO DE ESTUDIO" sheetId="16" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="79">
   <si>
     <t>FICHA</t>
   </si>
@@ -159,9 +159,6 @@
     <t>Identifica los elementos de la intersección</t>
   </si>
   <si>
-    <t>Actividad para prcticar la diferencia entre conjuntos</t>
-  </si>
-  <si>
     <t>Refuerza tu aprendizaje: Operaciones entre conjuntos</t>
   </si>
   <si>
@@ -219,9 +216,6 @@
     <t>Recuerda</t>
   </si>
   <si>
-    <t xml:space="preserve">Refuerza tu aprendizaje: Relación de pertenencia y contenencia. </t>
-  </si>
-  <si>
     <t xml:space="preserve">¿Cuál conjunto está contenido? </t>
   </si>
   <si>
@@ -240,9 +234,6 @@
     <t>Conjunto vacío</t>
   </si>
   <si>
-    <t xml:space="preserve">Refuerza tu aprendizaje: Clasificación de conjuntos. </t>
-  </si>
-  <si>
     <t>Operaciones entre conjuntos</t>
   </si>
   <si>
@@ -252,18 +243,12 @@
     <t>Intersección entre conjuntos</t>
   </si>
   <si>
-    <t>Identifica los objetos de la intersección</t>
-  </si>
-  <si>
     <t>Diferencia entre conjuntos</t>
   </si>
   <si>
     <t>Ejercitación y competencias</t>
   </si>
   <si>
-    <t xml:space="preserve">Refuerza tu aprendizaje: Conjuntos. </t>
-  </si>
-  <si>
     <t>Fin de la unidad</t>
   </si>
   <si>
@@ -279,10 +264,10 @@
     <t>Refuerza tu aprendizaje: Identifica conjuntos</t>
   </si>
   <si>
-    <t>Resuelve problemas aplicando operaciones entre conjuntos.</t>
-  </si>
-  <si>
-    <t>Refiuerza tu aprendizaje: Resuelve problemas aplicando operaciones entre conjuntos.</t>
+    <t>Refuerza tu aprendizaje: Clasificación de conjuntos</t>
+  </si>
+  <si>
+    <t>Actividad para practicar la diferencia entre conjuntos</t>
   </si>
 </sst>
 </file>
@@ -845,7 +830,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -906,6 +891,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="401">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -1598,17 +1584,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="127.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.3984375" customWidth="1"/>
+    <col min="2" max="2" width="127.3984375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="13" t="s">
         <v>8</v>
       </c>
@@ -1616,7 +1602,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="13" t="s">
         <v>9</v>
       </c>
@@ -1624,7 +1610,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="13" t="s">
         <v>10</v>
       </c>
@@ -1632,7 +1618,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="13" t="s">
         <v>11</v>
       </c>
@@ -1640,7 +1626,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="13" t="s">
         <v>1</v>
       </c>
@@ -1648,7 +1634,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="13" t="s">
         <v>12</v>
       </c>
@@ -1675,19 +1661,19 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.7109375" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.73046875" customWidth="1"/>
+    <col min="5" max="5" width="20.3984375" customWidth="1"/>
+    <col min="7" max="7" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.73046875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
@@ -1707,7 +1693,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2"/>
@@ -1721,16 +1707,16 @@
       <c r="K2"/>
       <c r="L2"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="G12" s="8"/>
     </row>
   </sheetData>
@@ -1746,19 +1732,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="78.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="66.1328125" customWidth="1"/>
+    <col min="2" max="2" width="14.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
@@ -1769,7 +1755,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1780,7 +1766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1791,7 +1777,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -1802,7 +1788,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1813,7 +1799,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1824,7 +1810,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -1835,7 +1821,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
         <v>32</v>
       </c>
@@ -1846,7 +1832,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -1857,9 +1843,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>26</v>
@@ -1868,7 +1854,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -1879,7 +1865,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -1890,7 +1876,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -1901,7 +1887,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -1912,7 +1898,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -1923,7 +1909,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
         <v>39</v>
       </c>
@@ -1934,7 +1920,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="4" t="s">
         <v>40</v>
       </c>
@@ -1945,7 +1931,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -1956,9 +1942,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>42</v>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A19" s="31" t="s">
+        <v>78</v>
       </c>
       <c r="B19" t="s">
         <v>26</v>
@@ -1967,9 +1953,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" s="31" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B20" t="s">
         <v>28</v>
@@ -1978,9 +1964,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B21" t="s">
         <v>26</v>
@@ -1989,31 +1975,31 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>83</v>
-      </c>
-      <c r="B22" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A22" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="4">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A23" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
         <v>45</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" s="4">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="31" t="s">
-        <v>81</v>
       </c>
       <c r="B24" t="s">
         <v>26</v>
@@ -2022,7 +2008,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -2031,17 +2017,6 @@
       </c>
       <c r="C25">
         <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -2049,7 +2024,7 @@
     <sortCondition ref="C2:C65"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2066,17 +2041,17 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="92.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.265625" customWidth="1"/>
+    <col min="3" max="3" width="19.265625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="23.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
@@ -2087,7 +2062,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2098,7 +2073,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2109,7 +2084,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2120,7 +2095,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2131,7 +2106,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2142,7 +2117,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2153,7 +2128,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2164,7 +2139,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2175,18 +2150,18 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2197,7 +2172,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2208,7 +2183,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2219,7 +2194,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2230,7 +2205,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2241,7 +2216,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2252,7 +2227,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2263,7 +2238,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2274,84 +2249,84 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>42</v>
+      <c r="B19" s="31" t="s">
+        <v>78</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>43</v>
+      <c r="B20" s="31" t="s">
+        <v>75</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>45</v>
+      <c r="B23" s="31" t="s">
+        <v>76</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C27" s="6"/>
     </row>
   </sheetData>
@@ -2371,24 +2346,24 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I62"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="43.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="61.28515625" style="3" customWidth="1"/>
-    <col min="5" max="7" width="17.85546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="64.140625" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.1328125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="28.265625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="61.265625" style="3" customWidth="1"/>
+    <col min="5" max="7" width="17.86328125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="64.1328125" customWidth="1"/>
+    <col min="9" max="9" width="17.3984375" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="9" t="s">
         <v>6</v>
       </c>
@@ -2417,15 +2392,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>48</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>49</v>
       </c>
       <c r="D2" s="16"/>
       <c r="E2" s="16"/>
@@ -2434,15 +2409,15 @@
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D3" s="16"/>
       <c r="E3" s="16"/>
@@ -2451,15 +2426,15 @@
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>48</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>49</v>
       </c>
       <c r="D4" s="16"/>
       <c r="E4" s="16"/>
@@ -2468,57 +2443,57 @@
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="16" t="s">
         <v>50</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>51</v>
       </c>
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
@@ -2529,57 +2504,57 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
@@ -2590,57 +2565,57 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="16" t="s">
         <v>54</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>55</v>
       </c>
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
@@ -2651,19 +2626,19 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
@@ -2674,15 +2649,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D15" s="19"/>
       <c r="E15" s="19"/>
@@ -2691,57 +2666,57 @@
       <c r="H15" s="17"/>
       <c r="I15" s="17"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C16" s="18"/>
       <c r="D16" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F16" s="19"/>
       <c r="G16" s="19"/>
       <c r="H16" s="17"/>
       <c r="I16" s="17"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C17" s="18"/>
       <c r="D17" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
       <c r="H17" s="17"/>
       <c r="I17" s="17"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C18" s="18"/>
       <c r="D18" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F18" s="19"/>
       <c r="G18" s="19"/>
@@ -2752,19 +2727,19 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C19" s="18"/>
       <c r="D19" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F19" s="19"/>
       <c r="G19" s="19"/>
@@ -2775,95 +2750,95 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C20" s="18"/>
       <c r="D20" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F20" s="19"/>
       <c r="G20" s="19"/>
       <c r="H20" s="17"/>
       <c r="I20" s="17"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C21" s="18"/>
       <c r="D21" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F21" s="19"/>
       <c r="G21" s="19"/>
       <c r="H21" s="17"/>
       <c r="I21" s="17"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C22" s="18"/>
       <c r="D22" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="19" t="s">
         <v>59</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>60</v>
       </c>
       <c r="F22" s="19"/>
       <c r="G22" s="19"/>
       <c r="H22" s="17"/>
       <c r="I22" s="17"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C23" s="18"/>
       <c r="D23" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F23" s="19"/>
       <c r="G23" s="19"/>
       <c r="H23" s="17"/>
       <c r="I23" s="17"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C24" s="18"/>
       <c r="D24" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F24" s="19"/>
       <c r="G24" s="19"/>
@@ -2874,61 +2849,61 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C25" s="18"/>
       <c r="D25" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F25" s="19"/>
       <c r="G25" s="19"/>
       <c r="H25" s="17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I25" s="17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C26" s="18"/>
       <c r="D26" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F26" s="19"/>
       <c r="G26" s="19"/>
-      <c r="H26" s="17" t="s">
+      <c r="H26" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="I26" s="17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A27" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="I26" s="17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" s="21" t="s">
-        <v>64</v>
-      </c>
       <c r="C27" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
@@ -2937,15 +2912,15 @@
       <c r="H27" s="20"/>
       <c r="I27" s="20"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
@@ -2958,57 +2933,57 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C29" s="21"/>
       <c r="D29" s="22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
       <c r="H29" s="20"/>
       <c r="I29" s="20"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B30" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C30" s="21"/>
       <c r="D30" s="22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F30" s="22"/>
       <c r="G30" s="22"/>
       <c r="H30" s="20"/>
       <c r="I30" s="20"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C31" s="21"/>
       <c r="D31" s="22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F31" s="22"/>
       <c r="G31" s="22"/>
@@ -3019,57 +2994,57 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C32" s="21"/>
       <c r="D32" s="22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F32" s="22"/>
       <c r="G32" s="22"/>
       <c r="H32" s="20"/>
       <c r="I32" s="20"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C33" s="21"/>
       <c r="D33" s="22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F33" s="22"/>
       <c r="G33" s="22"/>
       <c r="H33" s="20"/>
       <c r="I33" s="20"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C34" s="21"/>
       <c r="D34" s="22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F34" s="22"/>
       <c r="G34" s="22"/>
@@ -3080,57 +3055,57 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C35" s="21"/>
       <c r="D35" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F35" s="22"/>
       <c r="G35" s="22"/>
       <c r="H35" s="20"/>
       <c r="I35" s="20"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C36" s="21"/>
       <c r="D36" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F36" s="22"/>
       <c r="G36" s="22"/>
       <c r="H36" s="20"/>
       <c r="I36" s="20"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C37" s="21"/>
       <c r="D37" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F37" s="22"/>
       <c r="G37" s="22"/>
@@ -3141,76 +3116,76 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C38" s="21"/>
       <c r="D38" s="22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F38" s="22"/>
       <c r="G38" s="22"/>
       <c r="H38" s="20"/>
       <c r="I38" s="20"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C39" s="21"/>
       <c r="D39" s="22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F39" s="22"/>
       <c r="G39" s="22"/>
       <c r="H39" s="20"/>
       <c r="I39" s="20"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A40" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C40" s="21"/>
       <c r="D40" s="22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E40" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F40" s="22"/>
       <c r="G40" s="22"/>
       <c r="H40" s="20"/>
       <c r="I40" s="20"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C41" s="21"/>
       <c r="D41" s="22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F41" s="22"/>
       <c r="G41" s="22"/>
@@ -3221,101 +3196,101 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C42" s="21"/>
       <c r="D42" s="22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E42" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F42" s="22"/>
       <c r="G42" s="22"/>
       <c r="H42" s="20"/>
       <c r="I42" s="20"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C43" s="21"/>
       <c r="D43" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E43" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F43" s="22"/>
       <c r="G43" s="22"/>
-      <c r="H43" s="20" t="s">
-        <v>69</v>
+      <c r="H43" s="32" t="s">
+        <v>77</v>
       </c>
       <c r="I43" s="20" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B44" s="24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C44" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D44" s="25" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E44" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F44" s="25"/>
       <c r="G44" s="25"/>
       <c r="H44" s="23"/>
       <c r="I44" s="23"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B45" s="24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C45" s="24"/>
       <c r="D45" s="25" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E45" s="25" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F45" s="25"/>
       <c r="G45" s="25"/>
       <c r="H45" s="23"/>
       <c r="I45" s="23"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A46" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B46" s="24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C46" s="24"/>
       <c r="D46" s="25" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E46" s="25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F46" s="25"/>
       <c r="G46" s="25"/>
@@ -3326,333 +3301,293 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B47" s="24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C47" s="24"/>
       <c r="D47" s="25" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E47" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F47" s="25"/>
       <c r="G47" s="25"/>
       <c r="H47" s="23"/>
       <c r="I47" s="23"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B48" s="24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C48" s="24"/>
       <c r="D48" s="25" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E48" s="25" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F48" s="25"/>
       <c r="G48" s="25"/>
       <c r="H48" s="23"/>
       <c r="I48" s="23"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B49" s="24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C49" s="24"/>
       <c r="D49" s="25" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E49" s="25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F49" s="25"/>
       <c r="G49" s="25"/>
-      <c r="H49" s="23" t="s">
-        <v>73</v>
+      <c r="H49" s="32" t="s">
+        <v>41</v>
       </c>
       <c r="I49" s="23" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B50" s="24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C50" s="24"/>
       <c r="D50" s="25" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E50" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F50" s="25"/>
       <c r="G50" s="25"/>
       <c r="H50" s="23"/>
       <c r="I50" s="23"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B51" s="24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C51" s="24"/>
       <c r="D51" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="E51" s="25" t="s">
         <v>74</v>
-      </c>
-      <c r="E51" s="25" t="s">
-        <v>79</v>
       </c>
       <c r="F51" s="25"/>
       <c r="G51" s="25"/>
       <c r="H51" s="23"/>
       <c r="I51" s="23"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B52" s="24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C52" s="24"/>
       <c r="D52" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="E52" s="25" t="s">
         <v>74</v>
-      </c>
-      <c r="E52" s="25" t="s">
-        <v>79</v>
       </c>
       <c r="F52" s="25"/>
       <c r="G52" s="25"/>
       <c r="H52" s="23"/>
       <c r="I52" s="23"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A53" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B53" s="24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C53" s="24"/>
       <c r="D53" s="25" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E53" s="25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F53" s="25"/>
       <c r="G53" s="25"/>
       <c r="H53" s="23"/>
       <c r="I53" s="23"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A54" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B54" s="24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C54" s="24"/>
       <c r="D54" s="25" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E54" s="25" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="F54" s="25"/>
       <c r="G54" s="25"/>
-      <c r="H54" s="23"/>
-      <c r="I54" s="23"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H54" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="I54" s="23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A55" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B55" s="24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C55" s="24"/>
       <c r="D55" s="25" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="E55" s="25" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F55" s="25"/>
       <c r="G55" s="25"/>
-      <c r="H55" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="I55" s="23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H55" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="I55" s="25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A56" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B56" s="24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C56" s="24"/>
       <c r="D56" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E56" s="25" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F56" s="25"/>
       <c r="G56" s="25"/>
       <c r="H56" s="23" t="s">
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="I56" s="25" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="B57" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="C57" s="24"/>
-      <c r="D57" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="E57" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="F57" s="25"/>
-      <c r="G57" s="25"/>
-      <c r="H57" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="I57" s="25"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="B58" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="C58" s="24"/>
-      <c r="D58" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="E58" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="F58" s="25"/>
-      <c r="G58" s="25"/>
-      <c r="H58" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="I58" s="25" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="B59" s="27" t="s">
-        <v>75</v>
-      </c>
-      <c r="C59" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="D59" s="28"/>
-      <c r="E59" s="28"/>
-      <c r="F59" s="28"/>
-      <c r="G59" s="28"/>
-      <c r="H59" s="26" t="s">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A57" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B57" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C57" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="D57" s="28"/>
+      <c r="E57" s="28"/>
+      <c r="F57" s="28"/>
+      <c r="G57" s="28"/>
+      <c r="H57" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="I57" s="26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A58" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B58" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C58" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="D58" s="28"/>
+      <c r="E58" s="28"/>
+      <c r="F58" s="28"/>
+      <c r="G58" s="28"/>
+      <c r="H58" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="I59" s="26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="B60" s="27" t="s">
-        <v>75</v>
-      </c>
-      <c r="C60" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="D60" s="28"/>
-      <c r="E60" s="28"/>
-      <c r="F60" s="28"/>
-      <c r="G60" s="28"/>
-      <c r="H60" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="I60" s="26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="B61" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="C61" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="D61" s="30"/>
-      <c r="E61" s="30"/>
-      <c r="F61" s="30"/>
-      <c r="G61" s="30"/>
-      <c r="H61" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="I61" s="29" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="B62" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="C62" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="D62" s="30"/>
-      <c r="E62" s="30"/>
-      <c r="F62" s="30"/>
-      <c r="G62" s="30"/>
-      <c r="H62" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="I62" s="29" t="s">
+      <c r="I58" s="26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A59" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B59" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="C59" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="D59" s="30"/>
+      <c r="E59" s="30"/>
+      <c r="F59" s="30"/>
+      <c r="G59" s="30"/>
+      <c r="H59" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="I59" s="29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A60" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B60" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="C60" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="D60" s="30"/>
+      <c r="E60" s="30"/>
+      <c r="F60" s="30"/>
+      <c r="G60" s="30"/>
+      <c r="H60" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="I60" s="29" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
MA0401: Ajustes de contenido
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado04/guion01/EsqueletoGuion_MA_04_01_CO.xlsx
+++ b/fuentes/contenidos/grado04/guion01/EsqueletoGuion_MA_04_01_CO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\Aula Planeta Colombia\Repositorios\Matematicas\fuentes\contenidos\grado04\guion01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Copia\JOHANNA\Documents\Documents\Matematicas\fuentes\contenidos\grado04\guion01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20492" windowHeight="7758" tabRatio="729"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="729" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="82">
   <si>
     <t>FICHA</t>
   </si>
@@ -268,6 +268,15 @@
   </si>
   <si>
     <t>Actividad para practicar la diferencia entre conjuntos</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: Resuelve problemas aplicando operaciones entre conjuntos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refuerza tu aprendizaje: Analiza operaciones entre conjuntos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refuerza tu aprendizaje: Operaciones entre conjuntos. </t>
   </si>
 </sst>
 </file>
@@ -1584,17 +1593,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.3984375" customWidth="1"/>
-    <col min="2" max="2" width="127.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="127.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>8</v>
       </c>
@@ -1602,7 +1611,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>9</v>
       </c>
@@ -1610,7 +1619,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>10</v>
       </c>
@@ -1618,7 +1627,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>11</v>
       </c>
@@ -1626,7 +1635,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>1</v>
       </c>
@@ -1634,7 +1643,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>12</v>
       </c>
@@ -1661,19 +1670,19 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.73046875" customWidth="1"/>
-    <col min="5" max="5" width="20.3984375" customWidth="1"/>
-    <col min="7" max="7" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.1328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.73046875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
@@ -1693,7 +1702,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2"/>
@@ -1707,16 +1716,16 @@
       <c r="K2"/>
       <c r="L2"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G12" s="8"/>
     </row>
   </sheetData>
@@ -1732,19 +1741,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="66.1328125" customWidth="1"/>
-    <col min="2" max="2" width="14.73046875" customWidth="1"/>
+    <col min="1" max="1" width="77.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
@@ -1755,7 +1764,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1766,7 +1775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1777,7 +1786,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -1788,7 +1797,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1799,7 +1808,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1810,7 +1819,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -1821,7 +1830,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>32</v>
       </c>
@@ -1832,7 +1841,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -1843,7 +1852,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>43</v>
       </c>
@@ -1854,7 +1863,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -1865,7 +1874,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -1876,7 +1885,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -1887,7 +1896,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -1898,7 +1907,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -1909,7 +1918,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>39</v>
       </c>
@@ -1920,7 +1929,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>40</v>
       </c>
@@ -1931,7 +1940,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -1942,7 +1951,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
         <v>78</v>
       </c>
@@ -1953,7 +1962,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
         <v>75</v>
       </c>
@@ -1964,7 +1973,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -1975,31 +1984,31 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A22" s="4" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="4">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A23" s="31" t="s">
+      <c r="B23" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="31" t="s">
         <v>76</v>
-      </c>
-      <c r="B23" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
-        <v>45</v>
       </c>
       <c r="B24" t="s">
         <v>26</v>
@@ -2008,15 +2017,26 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B25" t="s">
         <v>26</v>
       </c>
       <c r="C25">
         <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -2024,7 +2044,7 @@
     <sortCondition ref="C2:C65"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2044,14 +2064,14 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="92.265625" customWidth="1"/>
-    <col min="3" max="3" width="19.265625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
@@ -2062,7 +2082,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2073,7 +2093,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2084,7 +2104,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2095,7 +2115,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2106,7 +2126,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2117,7 +2137,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2128,7 +2148,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2139,7 +2159,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2150,7 +2170,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2161,7 +2181,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2172,7 +2192,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2183,7 +2203,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2194,7 +2214,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2205,7 +2225,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2216,7 +2236,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2227,7 +2247,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2238,7 +2258,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2249,7 +2269,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2260,7 +2280,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2271,7 +2291,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2282,7 +2302,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2293,7 +2313,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2304,7 +2324,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2315,7 +2335,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2326,7 +2346,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C27" s="6"/>
     </row>
   </sheetData>
@@ -2346,24 +2366,24 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.73046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.1328125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="28.265625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="61.265625" style="3" customWidth="1"/>
-    <col min="5" max="7" width="17.86328125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="64.1328125" customWidth="1"/>
-    <col min="9" max="9" width="17.3984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="61.28515625" style="3" customWidth="1"/>
+    <col min="5" max="7" width="17.85546875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="79.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>6</v>
       </c>
@@ -2392,7 +2412,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>19</v>
       </c>
@@ -2409,7 +2429,7 @@
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>19</v>
       </c>
@@ -2426,7 +2446,7 @@
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>19</v>
       </c>
@@ -2443,7 +2463,7 @@
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>19</v>
       </c>
@@ -2462,7 +2482,7 @@
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>19</v>
       </c>
@@ -2481,7 +2501,7 @@
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>19</v>
       </c>
@@ -2504,7 +2524,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>19</v>
       </c>
@@ -2523,7 +2543,7 @@
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>19</v>
       </c>
@@ -2542,7 +2562,7 @@
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>19</v>
       </c>
@@ -2565,7 +2585,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>19</v>
       </c>
@@ -2584,7 +2604,7 @@
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>19</v>
       </c>
@@ -2603,7 +2623,7 @@
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>19</v>
       </c>
@@ -2626,7 +2646,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>19</v>
       </c>
@@ -2649,7 +2669,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>19</v>
       </c>
@@ -2666,7 +2686,7 @@
       <c r="H15" s="17"/>
       <c r="I15" s="17"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
         <v>19</v>
       </c>
@@ -2685,7 +2705,7 @@
       <c r="H16" s="17"/>
       <c r="I16" s="17"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
         <v>19</v>
       </c>
@@ -2704,7 +2724,7 @@
       <c r="H17" s="17"/>
       <c r="I17" s="17"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>19</v>
       </c>
@@ -2727,7 +2747,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>19</v>
       </c>
@@ -2750,7 +2770,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>19</v>
       </c>
@@ -2769,7 +2789,7 @@
       <c r="H20" s="17"/>
       <c r="I20" s="17"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
         <v>19</v>
       </c>
@@ -2788,7 +2808,7 @@
       <c r="H21" s="17"/>
       <c r="I21" s="17"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
         <v>19</v>
       </c>
@@ -2807,7 +2827,7 @@
       <c r="H22" s="17"/>
       <c r="I22" s="17"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>19</v>
       </c>
@@ -2826,7 +2846,7 @@
       <c r="H23" s="17"/>
       <c r="I23" s="17"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>19</v>
       </c>
@@ -2849,7 +2869,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
         <v>19</v>
       </c>
@@ -2872,7 +2892,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>19</v>
       </c>
@@ -2895,7 +2915,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
         <v>19</v>
       </c>
@@ -2912,7 +2932,7 @@
       <c r="H27" s="20"/>
       <c r="I27" s="20"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="20" t="s">
         <v>19</v>
       </c>
@@ -2933,7 +2953,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>19</v>
       </c>
@@ -2952,7 +2972,7 @@
       <c r="H29" s="20"/>
       <c r="I29" s="20"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
         <v>19</v>
       </c>
@@ -2971,7 +2991,7 @@
       <c r="H30" s="20"/>
       <c r="I30" s="20"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>19</v>
       </c>
@@ -2994,7 +3014,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="20" t="s">
         <v>19</v>
       </c>
@@ -3013,7 +3033,7 @@
       <c r="H32" s="20"/>
       <c r="I32" s="20"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
         <v>19</v>
       </c>
@@ -3032,7 +3052,7 @@
       <c r="H33" s="20"/>
       <c r="I33" s="20"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="20" t="s">
         <v>19</v>
       </c>
@@ -3055,7 +3075,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>19</v>
       </c>
@@ -3074,7 +3094,7 @@
       <c r="H35" s="20"/>
       <c r="I35" s="20"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="20" t="s">
         <v>19</v>
       </c>
@@ -3093,7 +3113,7 @@
       <c r="H36" s="20"/>
       <c r="I36" s="20"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>19</v>
       </c>
@@ -3116,7 +3136,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="20" t="s">
         <v>19</v>
       </c>
@@ -3135,7 +3155,7 @@
       <c r="H38" s="20"/>
       <c r="I38" s="20"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
         <v>19</v>
       </c>
@@ -3154,7 +3174,7 @@
       <c r="H39" s="20"/>
       <c r="I39" s="20"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="20" t="s">
         <v>19</v>
       </c>
@@ -3173,7 +3193,7 @@
       <c r="H40" s="20"/>
       <c r="I40" s="20"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="s">
         <v>19</v>
       </c>
@@ -3196,7 +3216,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="20" t="s">
         <v>19</v>
       </c>
@@ -3215,7 +3235,7 @@
       <c r="H42" s="20"/>
       <c r="I42" s="20"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="20" t="s">
         <v>19</v>
       </c>
@@ -3238,7 +3258,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="23" t="s">
         <v>19</v>
       </c>
@@ -3259,7 +3279,7 @@
       <c r="H44" s="23"/>
       <c r="I44" s="23"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="23" t="s">
         <v>19</v>
       </c>
@@ -3278,7 +3298,7 @@
       <c r="H45" s="23"/>
       <c r="I45" s="23"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="23" t="s">
         <v>19</v>
       </c>
@@ -3301,7 +3321,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="23" t="s">
         <v>19</v>
       </c>
@@ -3320,7 +3340,7 @@
       <c r="H47" s="23"/>
       <c r="I47" s="23"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="23" t="s">
         <v>19</v>
       </c>
@@ -3339,7 +3359,7 @@
       <c r="H48" s="23"/>
       <c r="I48" s="23"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="23" t="s">
         <v>19</v>
       </c>
@@ -3362,7 +3382,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="23" t="s">
         <v>19</v>
       </c>
@@ -3381,7 +3401,7 @@
       <c r="H50" s="23"/>
       <c r="I50" s="23"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="23" t="s">
         <v>19</v>
       </c>
@@ -3400,7 +3420,7 @@
       <c r="H51" s="23"/>
       <c r="I51" s="23"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="23" t="s">
         <v>19</v>
       </c>
@@ -3419,7 +3439,7 @@
       <c r="H52" s="23"/>
       <c r="I52" s="23"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="23" t="s">
         <v>19</v>
       </c>
@@ -3438,7 +3458,7 @@
       <c r="H53" s="23"/>
       <c r="I53" s="23"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="23" t="s">
         <v>19</v>
       </c>
@@ -3461,7 +3481,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="23" t="s">
         <v>19</v>
       </c>
@@ -3478,13 +3498,13 @@
       <c r="F55" s="25"/>
       <c r="G55" s="25"/>
       <c r="H55" s="32" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="I55" s="25" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="23" t="s">
         <v>19</v>
       </c>
@@ -3500,35 +3520,37 @@
       </c>
       <c r="F56" s="25"/>
       <c r="G56" s="25"/>
-      <c r="H56" s="23" t="s">
-        <v>42</v>
+      <c r="H56" s="32" t="s">
+        <v>81</v>
       </c>
       <c r="I56" s="25" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A57" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="B57" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="C57" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="D57" s="28"/>
-      <c r="E57" s="28"/>
-      <c r="F57" s="28"/>
-      <c r="G57" s="28"/>
-      <c r="H57" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="I57" s="26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B57" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C57" s="24"/>
+      <c r="D57" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="E57" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="F57" s="25"/>
+      <c r="G57" s="25"/>
+      <c r="H57" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="I57" s="25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="26" t="s">
         <v>19</v>
       </c>
@@ -3542,35 +3564,35 @@
       <c r="E58" s="28"/>
       <c r="F58" s="28"/>
       <c r="G58" s="28"/>
-      <c r="H58" s="32" t="s">
+      <c r="H58" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="I58" s="26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B59" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C59" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="D59" s="28"/>
+      <c r="E59" s="28"/>
+      <c r="F59" s="28"/>
+      <c r="G59" s="28"/>
+      <c r="H59" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="I58" s="26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A59" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="B59" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="C59" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="D59" s="30"/>
-      <c r="E59" s="30"/>
-      <c r="F59" s="30"/>
-      <c r="G59" s="30"/>
-      <c r="H59" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="I59" s="29" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="I59" s="26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="29" t="s">
         <v>19</v>
       </c>
@@ -3578,16 +3600,37 @@
         <v>72</v>
       </c>
       <c r="C60" s="29" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="D60" s="30"/>
       <c r="E60" s="30"/>
       <c r="F60" s="30"/>
       <c r="G60" s="30"/>
       <c r="H60" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="I60" s="29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B61" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="C61" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="I60" s="29" t="s">
+      <c r="D61" s="30"/>
+      <c r="E61" s="30"/>
+      <c r="F61" s="30"/>
+      <c r="G61" s="30"/>
+      <c r="H61" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="I61" s="29" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
MA0401: Eliminación de punto al final de nombre de recurso
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado04/guion01/EsqueletoGuion_MA_04_01_CO.xlsx
+++ b/fuentes/contenidos/grado04/guion01/EsqueletoGuion_MA_04_01_CO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Copia\JOHANNA\Documents\Documents\Matematicas\fuentes\contenidos\grado04\guion01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Documents\Aula Planeta Colombia\Repositorios\Matematicas\fuentes\contenidos\grado04\guion01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="729" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20492" windowHeight="7758" tabRatio="729" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="81">
   <si>
     <t>FICHA</t>
   </si>
@@ -274,9 +274,6 @@
   </si>
   <si>
     <t xml:space="preserve">Refuerza tu aprendizaje: Analiza operaciones entre conjuntos </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Refuerza tu aprendizaje: Operaciones entre conjuntos. </t>
   </si>
 </sst>
 </file>
@@ -1597,13 +1594,13 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="127.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.3984375" customWidth="1"/>
+    <col min="2" max="2" width="127.3984375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="13" t="s">
         <v>8</v>
       </c>
@@ -1611,7 +1608,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="13" t="s">
         <v>9</v>
       </c>
@@ -1619,7 +1616,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="13" t="s">
         <v>10</v>
       </c>
@@ -1627,7 +1624,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="13" t="s">
         <v>11</v>
       </c>
@@ -1635,7 +1632,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="13" t="s">
         <v>1</v>
       </c>
@@ -1643,7 +1640,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="13" t="s">
         <v>12</v>
       </c>
@@ -1670,19 +1667,19 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.7109375" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.73046875" customWidth="1"/>
+    <col min="5" max="5" width="20.3984375" customWidth="1"/>
+    <col min="7" max="7" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.73046875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
@@ -1702,7 +1699,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2"/>
@@ -1716,16 +1713,16 @@
       <c r="K2"/>
       <c r="L2"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="G12" s="8"/>
     </row>
   </sheetData>
@@ -1747,13 +1744,13 @@
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="77.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="77.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
@@ -1764,7 +1761,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1775,7 +1772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1786,7 +1783,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -1797,7 +1794,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1808,7 +1805,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1819,7 +1816,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -1830,7 +1827,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
         <v>32</v>
       </c>
@@ -1841,7 +1838,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -1852,7 +1849,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
         <v>43</v>
       </c>
@@ -1863,7 +1860,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -1874,7 +1871,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -1885,7 +1882,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -1896,7 +1893,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -1907,7 +1904,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -1918,7 +1915,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
         <v>39</v>
       </c>
@@ -1929,7 +1926,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="4" t="s">
         <v>40</v>
       </c>
@@ -1940,7 +1937,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -1951,7 +1948,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="31" t="s">
         <v>78</v>
       </c>
@@ -1962,7 +1959,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" s="31" t="s">
         <v>75</v>
       </c>
@@ -1973,7 +1970,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -1984,7 +1981,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>79</v>
       </c>
@@ -1995,7 +1992,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="4" t="s">
         <v>44</v>
       </c>
@@ -2006,7 +2003,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="31" t="s">
         <v>76</v>
       </c>
@@ -2017,7 +2014,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>45</v>
       </c>
@@ -2028,7 +2025,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>46</v>
       </c>
@@ -2061,17 +2058,17 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="92.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.265625" customWidth="1"/>
+    <col min="3" max="3" width="19.265625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="23.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
@@ -2082,7 +2079,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2093,7 +2090,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2104,7 +2101,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2115,7 +2112,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2126,7 +2123,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2137,7 +2134,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2148,7 +2145,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2159,7 +2156,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2170,7 +2167,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2181,7 +2178,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2192,7 +2189,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2203,7 +2200,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2214,7 +2211,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2225,7 +2222,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2236,7 +2233,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2247,7 +2244,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2258,7 +2255,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2269,7 +2266,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2280,7 +2277,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2291,7 +2288,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2302,7 +2299,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2313,7 +2310,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2324,7 +2321,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2335,7 +2332,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2346,7 +2343,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C27" s="6"/>
     </row>
   </sheetData>
@@ -2368,22 +2365,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="H58" sqref="H58"/>
+    <sheetView tabSelected="1" topLeftCell="C27" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="43.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="61.28515625" style="3" customWidth="1"/>
-    <col min="5" max="7" width="17.85546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="79.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.1328125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="28.265625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="61.265625" style="3" customWidth="1"/>
+    <col min="5" max="7" width="17.86328125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="79.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.3984375" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="9" t="s">
         <v>6</v>
       </c>
@@ -2412,7 +2409,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="14" t="s">
         <v>19</v>
       </c>
@@ -2429,7 +2426,7 @@
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="14" t="s">
         <v>19</v>
       </c>
@@ -2446,7 +2443,7 @@
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="14" t="s">
         <v>19</v>
       </c>
@@ -2463,7 +2460,7 @@
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="14" t="s">
         <v>19</v>
       </c>
@@ -2482,7 +2479,7 @@
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="14" t="s">
         <v>19</v>
       </c>
@@ -2501,7 +2498,7 @@
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="14" t="s">
         <v>19</v>
       </c>
@@ -2524,7 +2521,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="14" t="s">
         <v>19</v>
       </c>
@@ -2543,7 +2540,7 @@
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="14" t="s">
         <v>19</v>
       </c>
@@ -2562,7 +2559,7 @@
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="14" t="s">
         <v>19</v>
       </c>
@@ -2585,7 +2582,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="14" t="s">
         <v>19</v>
       </c>
@@ -2604,7 +2601,7 @@
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="14" t="s">
         <v>19</v>
       </c>
@@ -2623,7 +2620,7 @@
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="14" t="s">
         <v>19</v>
       </c>
@@ -2646,7 +2643,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="14" t="s">
         <v>19</v>
       </c>
@@ -2669,7 +2666,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="17" t="s">
         <v>19</v>
       </c>
@@ -2686,7 +2683,7 @@
       <c r="H15" s="17"/>
       <c r="I15" s="17"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="17" t="s">
         <v>19</v>
       </c>
@@ -2705,7 +2702,7 @@
       <c r="H16" s="17"/>
       <c r="I16" s="17"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="17" t="s">
         <v>19</v>
       </c>
@@ -2724,7 +2721,7 @@
       <c r="H17" s="17"/>
       <c r="I17" s="17"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="17" t="s">
         <v>19</v>
       </c>
@@ -2747,7 +2744,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="17" t="s">
         <v>19</v>
       </c>
@@ -2770,7 +2767,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="17" t="s">
         <v>19</v>
       </c>
@@ -2789,7 +2786,7 @@
       <c r="H20" s="17"/>
       <c r="I20" s="17"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="17" t="s">
         <v>19</v>
       </c>
@@ -2808,7 +2805,7 @@
       <c r="H21" s="17"/>
       <c r="I21" s="17"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="17" t="s">
         <v>19</v>
       </c>
@@ -2827,7 +2824,7 @@
       <c r="H22" s="17"/>
       <c r="I22" s="17"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="17" t="s">
         <v>19</v>
       </c>
@@ -2846,7 +2843,7 @@
       <c r="H23" s="17"/>
       <c r="I23" s="17"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="17" t="s">
         <v>19</v>
       </c>
@@ -2869,7 +2866,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="17" t="s">
         <v>19</v>
       </c>
@@ -2892,7 +2889,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="17" t="s">
         <v>19</v>
       </c>
@@ -2915,7 +2912,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" s="20" t="s">
         <v>19</v>
       </c>
@@ -2932,7 +2929,7 @@
       <c r="H27" s="20"/>
       <c r="I27" s="20"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" s="20" t="s">
         <v>19</v>
       </c>
@@ -2953,7 +2950,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" s="20" t="s">
         <v>19</v>
       </c>
@@ -2972,7 +2969,7 @@
       <c r="H29" s="20"/>
       <c r="I29" s="20"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" s="20" t="s">
         <v>19</v>
       </c>
@@ -2991,7 +2988,7 @@
       <c r="H30" s="20"/>
       <c r="I30" s="20"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" s="20" t="s">
         <v>19</v>
       </c>
@@ -3014,7 +3011,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" s="20" t="s">
         <v>19</v>
       </c>
@@ -3033,7 +3030,7 @@
       <c r="H32" s="20"/>
       <c r="I32" s="20"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" s="20" t="s">
         <v>19</v>
       </c>
@@ -3052,7 +3049,7 @@
       <c r="H33" s="20"/>
       <c r="I33" s="20"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34" s="20" t="s">
         <v>19</v>
       </c>
@@ -3075,7 +3072,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" s="20" t="s">
         <v>19</v>
       </c>
@@ -3094,7 +3091,7 @@
       <c r="H35" s="20"/>
       <c r="I35" s="20"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" s="20" t="s">
         <v>19</v>
       </c>
@@ -3113,7 +3110,7 @@
       <c r="H36" s="20"/>
       <c r="I36" s="20"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" s="20" t="s">
         <v>19</v>
       </c>
@@ -3136,7 +3133,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" s="20" t="s">
         <v>19</v>
       </c>
@@ -3155,7 +3152,7 @@
       <c r="H38" s="20"/>
       <c r="I38" s="20"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39" s="20" t="s">
         <v>19</v>
       </c>
@@ -3174,7 +3171,7 @@
       <c r="H39" s="20"/>
       <c r="I39" s="20"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A40" s="20" t="s">
         <v>19</v>
       </c>
@@ -3193,7 +3190,7 @@
       <c r="H40" s="20"/>
       <c r="I40" s="20"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41" s="20" t="s">
         <v>19</v>
       </c>
@@ -3216,7 +3213,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42" s="20" t="s">
         <v>19</v>
       </c>
@@ -3235,7 +3232,7 @@
       <c r="H42" s="20"/>
       <c r="I42" s="20"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43" s="20" t="s">
         <v>19</v>
       </c>
@@ -3258,7 +3255,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" s="23" t="s">
         <v>19</v>
       </c>
@@ -3279,7 +3276,7 @@
       <c r="H44" s="23"/>
       <c r="I44" s="23"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45" s="23" t="s">
         <v>19</v>
       </c>
@@ -3298,7 +3295,7 @@
       <c r="H45" s="23"/>
       <c r="I45" s="23"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A46" s="23" t="s">
         <v>19</v>
       </c>
@@ -3321,7 +3318,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47" s="23" t="s">
         <v>19</v>
       </c>
@@ -3340,7 +3337,7 @@
       <c r="H47" s="23"/>
       <c r="I47" s="23"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48" s="23" t="s">
         <v>19</v>
       </c>
@@ -3359,7 +3356,7 @@
       <c r="H48" s="23"/>
       <c r="I48" s="23"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" s="23" t="s">
         <v>19</v>
       </c>
@@ -3382,7 +3379,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" s="23" t="s">
         <v>19</v>
       </c>
@@ -3401,7 +3398,7 @@
       <c r="H50" s="23"/>
       <c r="I50" s="23"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" s="23" t="s">
         <v>19</v>
       </c>
@@ -3420,7 +3417,7 @@
       <c r="H51" s="23"/>
       <c r="I51" s="23"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" s="23" t="s">
         <v>19</v>
       </c>
@@ -3439,7 +3436,7 @@
       <c r="H52" s="23"/>
       <c r="I52" s="23"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A53" s="23" t="s">
         <v>19</v>
       </c>
@@ -3458,7 +3455,7 @@
       <c r="H53" s="23"/>
       <c r="I53" s="23"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A54" s="23" t="s">
         <v>19</v>
       </c>
@@ -3481,7 +3478,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A55" s="23" t="s">
         <v>19</v>
       </c>
@@ -3504,7 +3501,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A56" s="23" t="s">
         <v>19</v>
       </c>
@@ -3521,13 +3518,13 @@
       <c r="F56" s="25"/>
       <c r="G56" s="25"/>
       <c r="H56" s="32" t="s">
-        <v>81</v>
+        <v>42</v>
       </c>
       <c r="I56" s="25" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A57" s="23" t="s">
         <v>19</v>
       </c>
@@ -3550,7 +3547,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A58" s="26" t="s">
         <v>19</v>
       </c>
@@ -3571,7 +3568,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A59" s="26" t="s">
         <v>19</v>
       </c>
@@ -3592,7 +3589,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A60" s="29" t="s">
         <v>19</v>
       </c>
@@ -3613,7 +3610,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A61" s="29" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Matemática 6 Tema 1
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado04/guion01/EsqueletoGuion_MA_04_01_CO.xlsx
+++ b/fuentes/contenidos/grado04/guion01/EsqueletoGuion_MA_04_01_CO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Documents\Aula Planeta Colombia\Repositorios\Matematicas\fuentes\contenidos\grado04\guion01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DianaMargarita\Documents\GitHub\Matematicas\fuentes\contenidos\grado04\guion01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20492" windowHeight="7758" tabRatio="729" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="729" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="RECURSOS NUEVOS" sheetId="13" r:id="rId3"/>
     <sheet name="CUADERNO DEL PROFESOR" sheetId="15" r:id="rId4"/>
     <sheet name="CUADERNO DE ESTUDIO" sheetId="16" r:id="rId5"/>
+    <sheet name="Hoja1" sheetId="17" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -1591,16 +1592,16 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.3984375" customWidth="1"/>
-    <col min="2" max="2" width="127.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="127.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>8</v>
       </c>
@@ -1608,7 +1609,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>9</v>
       </c>
@@ -1616,7 +1617,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>10</v>
       </c>
@@ -1624,7 +1625,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>11</v>
       </c>
@@ -1632,7 +1633,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>1</v>
       </c>
@@ -1640,7 +1641,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>12</v>
       </c>
@@ -1664,22 +1665,22 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.73046875" customWidth="1"/>
-    <col min="5" max="5" width="20.3984375" customWidth="1"/>
-    <col min="7" max="7" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.1328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.73046875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
@@ -1699,7 +1700,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2"/>
@@ -1713,16 +1714,16 @@
       <c r="K2"/>
       <c r="L2"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G12" s="8"/>
     </row>
   </sheetData>
@@ -1740,17 +1741,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="77.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.73046875" customWidth="1"/>
+    <col min="1" max="1" width="77.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
@@ -1761,18 +1762,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="31" t="s">
         <v>26</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1783,7 +1784,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -1794,7 +1795,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1805,7 +1806,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1816,7 +1817,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -1827,7 +1828,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>32</v>
       </c>
@@ -1838,7 +1839,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -1849,7 +1850,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>43</v>
       </c>
@@ -1860,7 +1861,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -1871,7 +1872,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -1882,7 +1883,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -1893,7 +1894,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -1904,7 +1905,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -1915,7 +1916,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>39</v>
       </c>
@@ -1926,7 +1927,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>40</v>
       </c>
@@ -1937,7 +1938,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -1948,7 +1949,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
         <v>78</v>
       </c>
@@ -1959,7 +1960,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
         <v>75</v>
       </c>
@@ -1970,7 +1971,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -1981,7 +1982,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>79</v>
       </c>
@@ -1992,7 +1993,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>44</v>
       </c>
@@ -2003,7 +2004,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="31" t="s">
         <v>76</v>
       </c>
@@ -2014,7 +2015,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>45</v>
       </c>
@@ -2025,7 +2026,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>46</v>
       </c>
@@ -2058,17 +2059,17 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="92.265625" customWidth="1"/>
-    <col min="3" max="3" width="19.265625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
@@ -2079,7 +2080,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2090,7 +2091,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2101,7 +2102,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2112,7 +2113,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2123,7 +2124,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2134,7 +2135,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2145,7 +2146,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2156,7 +2157,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2167,7 +2168,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2178,7 +2179,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2189,7 +2190,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2200,7 +2201,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2211,7 +2212,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2222,7 +2223,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2233,7 +2234,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2244,7 +2245,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2255,7 +2256,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2266,7 +2267,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2277,7 +2278,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2288,7 +2289,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2299,7 +2300,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2310,7 +2311,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2321,7 +2322,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2332,7 +2333,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2343,7 +2344,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C27" s="6"/>
     </row>
   </sheetData>
@@ -2365,22 +2366,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C27" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="H57" sqref="H57"/>
+    <sheetView topLeftCell="C1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.73046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.1328125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="28.265625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="61.265625" style="3" customWidth="1"/>
-    <col min="5" max="7" width="17.86328125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="79.3984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.3984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="61.28515625" style="3" customWidth="1"/>
+    <col min="5" max="7" width="17.85546875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="79.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>6</v>
       </c>
@@ -2409,7 +2410,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>19</v>
       </c>
@@ -2426,7 +2427,7 @@
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>19</v>
       </c>
@@ -2443,7 +2444,7 @@
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>19</v>
       </c>
@@ -2460,7 +2461,7 @@
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>19</v>
       </c>
@@ -2479,7 +2480,7 @@
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>19</v>
       </c>
@@ -2498,7 +2499,7 @@
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>19</v>
       </c>
@@ -2521,7 +2522,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>19</v>
       </c>
@@ -2540,7 +2541,7 @@
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>19</v>
       </c>
@@ -2559,7 +2560,7 @@
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>19</v>
       </c>
@@ -2582,7 +2583,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>19</v>
       </c>
@@ -2601,7 +2602,7 @@
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>19</v>
       </c>
@@ -2620,7 +2621,7 @@
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>19</v>
       </c>
@@ -2643,7 +2644,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>19</v>
       </c>
@@ -2666,7 +2667,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>19</v>
       </c>
@@ -2683,7 +2684,7 @@
       <c r="H15" s="17"/>
       <c r="I15" s="17"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
         <v>19</v>
       </c>
@@ -2702,7 +2703,7 @@
       <c r="H16" s="17"/>
       <c r="I16" s="17"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
         <v>19</v>
       </c>
@@ -2721,7 +2722,7 @@
       <c r="H17" s="17"/>
       <c r="I17" s="17"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>19</v>
       </c>
@@ -2744,7 +2745,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>19</v>
       </c>
@@ -2767,7 +2768,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>19</v>
       </c>
@@ -2786,7 +2787,7 @@
       <c r="H20" s="17"/>
       <c r="I20" s="17"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
         <v>19</v>
       </c>
@@ -2805,7 +2806,7 @@
       <c r="H21" s="17"/>
       <c r="I21" s="17"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
         <v>19</v>
       </c>
@@ -2824,7 +2825,7 @@
       <c r="H22" s="17"/>
       <c r="I22" s="17"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>19</v>
       </c>
@@ -2843,7 +2844,7 @@
       <c r="H23" s="17"/>
       <c r="I23" s="17"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>19</v>
       </c>
@@ -2866,7 +2867,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
         <v>19</v>
       </c>
@@ -2889,7 +2890,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>19</v>
       </c>
@@ -2912,7 +2913,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
         <v>19</v>
       </c>
@@ -2929,7 +2930,7 @@
       <c r="H27" s="20"/>
       <c r="I27" s="20"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="20" t="s">
         <v>19</v>
       </c>
@@ -2950,7 +2951,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>19</v>
       </c>
@@ -2969,7 +2970,7 @@
       <c r="H29" s="20"/>
       <c r="I29" s="20"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
         <v>19</v>
       </c>
@@ -2988,7 +2989,7 @@
       <c r="H30" s="20"/>
       <c r="I30" s="20"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>19</v>
       </c>
@@ -3011,7 +3012,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="20" t="s">
         <v>19</v>
       </c>
@@ -3030,7 +3031,7 @@
       <c r="H32" s="20"/>
       <c r="I32" s="20"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
         <v>19</v>
       </c>
@@ -3049,7 +3050,7 @@
       <c r="H33" s="20"/>
       <c r="I33" s="20"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="20" t="s">
         <v>19</v>
       </c>
@@ -3072,7 +3073,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>19</v>
       </c>
@@ -3091,7 +3092,7 @@
       <c r="H35" s="20"/>
       <c r="I35" s="20"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="20" t="s">
         <v>19</v>
       </c>
@@ -3110,7 +3111,7 @@
       <c r="H36" s="20"/>
       <c r="I36" s="20"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>19</v>
       </c>
@@ -3133,7 +3134,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="20" t="s">
         <v>19</v>
       </c>
@@ -3152,7 +3153,7 @@
       <c r="H38" s="20"/>
       <c r="I38" s="20"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
         <v>19</v>
       </c>
@@ -3171,7 +3172,7 @@
       <c r="H39" s="20"/>
       <c r="I39" s="20"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="20" t="s">
         <v>19</v>
       </c>
@@ -3190,7 +3191,7 @@
       <c r="H40" s="20"/>
       <c r="I40" s="20"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="s">
         <v>19</v>
       </c>
@@ -3213,7 +3214,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="20" t="s">
         <v>19</v>
       </c>
@@ -3232,7 +3233,7 @@
       <c r="H42" s="20"/>
       <c r="I42" s="20"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="20" t="s">
         <v>19</v>
       </c>
@@ -3255,7 +3256,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="23" t="s">
         <v>19</v>
       </c>
@@ -3276,7 +3277,7 @@
       <c r="H44" s="23"/>
       <c r="I44" s="23"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="23" t="s">
         <v>19</v>
       </c>
@@ -3295,7 +3296,7 @@
       <c r="H45" s="23"/>
       <c r="I45" s="23"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="23" t="s">
         <v>19</v>
       </c>
@@ -3318,7 +3319,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="23" t="s">
         <v>19</v>
       </c>
@@ -3337,7 +3338,7 @@
       <c r="H47" s="23"/>
       <c r="I47" s="23"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="23" t="s">
         <v>19</v>
       </c>
@@ -3356,7 +3357,7 @@
       <c r="H48" s="23"/>
       <c r="I48" s="23"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="23" t="s">
         <v>19</v>
       </c>
@@ -3379,7 +3380,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="23" t="s">
         <v>19</v>
       </c>
@@ -3398,7 +3399,7 @@
       <c r="H50" s="23"/>
       <c r="I50" s="23"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="23" t="s">
         <v>19</v>
       </c>
@@ -3417,7 +3418,7 @@
       <c r="H51" s="23"/>
       <c r="I51" s="23"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="23" t="s">
         <v>19</v>
       </c>
@@ -3436,7 +3437,7 @@
       <c r="H52" s="23"/>
       <c r="I52" s="23"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="23" t="s">
         <v>19</v>
       </c>
@@ -3455,7 +3456,7 @@
       <c r="H53" s="23"/>
       <c r="I53" s="23"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="23" t="s">
         <v>19</v>
       </c>
@@ -3478,7 +3479,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="23" t="s">
         <v>19</v>
       </c>
@@ -3501,7 +3502,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="23" t="s">
         <v>19</v>
       </c>
@@ -3524,7 +3525,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="23" t="s">
         <v>19</v>
       </c>
@@ -3547,7 +3548,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="26" t="s">
         <v>19</v>
       </c>
@@ -3568,7 +3569,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="26" t="s">
         <v>19</v>
       </c>
@@ -3589,7 +3590,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="29" t="s">
         <v>19</v>
       </c>
@@ -3610,7 +3611,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="29" t="s">
         <v>19</v>
       </c>
@@ -3640,4 +3641,16 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>